<commit_message>
Atualização do Projeto de IA
</commit_message>
<xml_diff>
--- a/controle_financeiro.xlsx
+++ b/controle_financeiro.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -835,6 +835,156 @@
         <v>10</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>09/11/2025 00:06:05</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fundo emergencial </t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Guarde 300</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>outros</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>09/11/2025 00:06:44</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Saída</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Gastei 550</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>outros</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>09/11/2025 00:08:00</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Saída</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Gastei 300</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>outros</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>09/11/2025 00:08:53</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Saída</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Gastei 500</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>outros</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>11/11/2025 07:16:24</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Recebi 7000</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>outros</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>11/11/2025 07:16:55</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Recebi 2000</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>outros</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>2000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>